<commit_message>
fix arial bold font problem
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/books/currencyExchange.xlsx
+++ b/src/main/webapp/WEB-INF/books/currencyExchange.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/KEIKAI-SPACE/dev-ref/src/main/webapp/WEB-INF/books/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06EDD51F-4794-9148-9511-210C003ADBBD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14008A59-375B-274F-9D4F-54C61951C757}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="1060" windowWidth="33600" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33600" yWindow="1060" windowWidth="33600" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="select" sheetId="1" r:id="rId1"/>
@@ -110,7 +110,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$€-2]\ #,##0.00"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="19">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -231,14 +231,11 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
       <sz val="12"/>
       <color theme="1" tint="0.249977111117893"/>
-      <name val="Arial Bold"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial Bold"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -470,8 +467,6 @@
     <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
@@ -512,6 +507,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1114,21 +1111,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="83" customHeight="1">
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="65"/>
-      <c r="N2" s="65"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
+      <c r="N2" s="63"/>
     </row>
     <row r="3" spans="2:15" ht="6" customHeight="1">
       <c r="B3" s="16"/>
@@ -1163,32 +1160,32 @@
     </row>
     <row r="5" spans="2:15">
       <c r="B5" s="11"/>
-      <c r="C5" s="63"/>
+      <c r="C5" s="61"/>
       <c r="D5" s="11"/>
       <c r="E5" s="24"/>
-      <c r="F5" s="66" t="s">
+      <c r="F5" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="66"/>
-      <c r="H5" s="66"/>
-      <c r="I5" s="67"/>
-      <c r="J5" s="67"/>
-      <c r="K5" s="67"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="65"/>
+      <c r="J5" s="65"/>
+      <c r="K5" s="65"/>
       <c r="L5" s="26"/>
       <c r="M5" s="26"/>
       <c r="N5" s="10"/>
     </row>
     <row r="6" spans="2:15">
       <c r="B6" s="11"/>
-      <c r="C6" s="63"/>
+      <c r="C6" s="61"/>
       <c r="D6" s="11"/>
       <c r="E6" s="24"/>
-      <c r="F6" s="66"/>
-      <c r="G6" s="66"/>
-      <c r="H6" s="66"/>
-      <c r="I6" s="67"/>
-      <c r="J6" s="67"/>
-      <c r="K6" s="67"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="64"/>
+      <c r="H6" s="64"/>
+      <c r="I6" s="65"/>
+      <c r="J6" s="65"/>
+      <c r="K6" s="65"/>
       <c r="L6" s="26"/>
       <c r="M6" s="26"/>
       <c r="N6" s="10"/>
@@ -1758,8 +1755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:P18"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:K2"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -1778,18 +1775,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:16" ht="83" customHeight="1">
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62"/>
     </row>
     <row r="3" spans="1:16" ht="6" customHeight="1">
       <c r="A3" s="5"/>
@@ -1821,12 +1818,12 @@
     <row r="5" spans="1:16">
       <c r="B5" s="10"/>
       <c r="C5" s="24"/>
-      <c r="D5" s="68" t="s">
+      <c r="D5" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="68"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
@@ -1835,10 +1832,10 @@
     <row r="6" spans="1:16" ht="17" customHeight="1" thickBot="1">
       <c r="B6" s="10"/>
       <c r="C6" s="24"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
-      <c r="F6" s="68"/>
-      <c r="G6" s="68"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="66"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
@@ -1854,15 +1851,15 @@
       <c r="F7" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="G7" s="55">
+      <c r="G7" s="71">
         <f>D7*G9</f>
         <v>0</v>
       </c>
-      <c r="H7" s="56" t="str">
+      <c r="H7" s="72" t="str">
         <f>H9</f>
         <v>USD</v>
       </c>
-      <c r="I7" s="57"/>
+      <c r="I7" s="55"/>
       <c r="J7" s="48" t="s">
         <v>19</v>
       </c>
@@ -1871,19 +1868,19 @@
     <row r="8" spans="1:16" ht="10" customHeight="1">
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
-      <c r="D8" s="58"/>
-      <c r="E8" s="59"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="57"/>
       <c r="F8" s="46"/>
-      <c r="G8" s="60"/>
-      <c r="H8" s="61"/>
-      <c r="I8" s="57"/>
+      <c r="G8" s="58"/>
+      <c r="H8" s="59"/>
+      <c r="I8" s="55"/>
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
     </row>
     <row r="9" spans="1:16">
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
-      <c r="D9" s="61">
+      <c r="D9" s="59">
         <v>1</v>
       </c>
       <c r="E9" s="54" t="s">
@@ -1892,13 +1889,13 @@
       <c r="F9" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="G9" s="62">
+      <c r="G9" s="60">
         <v>1.1200000000000001</v>
       </c>
-      <c r="H9" s="61" t="s">
+      <c r="H9" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="I9" s="57"/>
+      <c r="I9" s="55"/>
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
     </row>
@@ -1964,19 +1961,19 @@
     </row>
     <row r="16" spans="1:16">
       <c r="B16" s="4"/>
-      <c r="C16" s="69"/>
-      <c r="D16" s="69"/>
-      <c r="E16" s="69"/>
-      <c r="F16" s="69"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="67"/>
       <c r="O16" s="42"/>
       <c r="P16" s="42"/>
     </row>
     <row r="17" spans="2:6">
       <c r="B17" s="3"/>
-      <c r="C17" s="69"/>
-      <c r="D17" s="69"/>
-      <c r="E17" s="69"/>
-      <c r="F17" s="69"/>
+      <c r="C17" s="67"/>
+      <c r="D17" s="67"/>
+      <c r="E17" s="67"/>
+      <c r="F17" s="67"/>
     </row>
     <row r="18" spans="2:6">
       <c r="B18" s="5"/>
@@ -2000,7 +1997,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:M15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
@@ -2022,19 +2019,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" ht="83" customHeight="1">
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="64"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62"/>
+      <c r="L2" s="62"/>
     </row>
     <row r="3" spans="1:13" ht="6" customHeight="1" thickBot="1">
       <c r="A3" s="5"/>
@@ -2058,11 +2055,11 @@
       <c r="F4" s="23"/>
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
-      <c r="I4" s="70" t="s">
+      <c r="I4" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="71"/>
-      <c r="K4" s="72"/>
+      <c r="J4" s="69"/>
+      <c r="K4" s="70"/>
       <c r="L4" s="10"/>
     </row>
     <row r="5" spans="1:13" ht="23" customHeight="1">

</xml_diff>